<commit_message>
test case pincode change
</commit_message>
<xml_diff>
--- a/src/test/resources/Sprint2.xlsx
+++ b/src/test/resources/Sprint2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AKASALKA\PumaSprint2\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akshata K\IdeaProjects\Sprint 2(Puma)\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0C7300-0A3D-4EDF-A343-0B2DB1C68445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DE09FE-B9F4-4BCC-BE0E-CAE54740319F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BCE4E5A8-B7C4-4A55-85EF-069713A2933F}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Scenario_name</t>
   </si>
@@ -51,6 +40,12 @@
   </si>
   <si>
     <t>Verify that user able to enter the  invalid pincode</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>5800  '</t>
   </si>
 </sst>
 </file>
@@ -100,7 +95,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -111,6 +106,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,27 +424,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{775B676E-DE4E-43E4-9CE3-A4F6948032A5}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="66.36328125" customWidth="1"/>
     <col min="2" max="2" width="20.54296875" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -453,16 +456,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>